<commit_message>
Se completó el código de la clase Punto2D y Punto3D.
</commit_message>
<xml_diff>
--- a/practica3/trunk/Jerarquias/doc/metricas.xlsx
+++ b/practica3/trunk/Jerarquias/doc/metricas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -92,16 +92,25 @@
   </si>
   <si>
     <t>TIEMPO EFECTIVO DESARROLLO</t>
+  </si>
+  <si>
+    <t>Implementacion de intefaz punto</t>
+  </si>
+  <si>
+    <t>Implementacion de Punto2D</t>
+  </si>
+  <si>
+    <t>Implementacion de Punto3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -781,13 +790,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="20% - Énfasis5" xfId="1" builtinId="46"/>
-    <cellStyle name="40% - Énfasis2" xfId="2" builtinId="35"/>
-    <cellStyle name="40% - Énfasis6" xfId="3" builtinId="51"/>
-    <cellStyle name="60% - Énfasis5" xfId="4" builtinId="48"/>
-    <cellStyle name="Énfasis2" xfId="5" builtinId="33"/>
-    <cellStyle name="Énfasis5" xfId="6" builtinId="45"/>
-    <cellStyle name="Énfasis6" xfId="7" builtinId="49"/>
+    <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
+    <cellStyle name="40% - Accent2" xfId="2" builtinId="35"/>
+    <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Accent5" xfId="6" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="7" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -870,17 +879,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -899,9 +899,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -911,7 +909,6 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -956,7 +953,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -1055,16 +1051,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-AR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1087,23 +1077,17 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.05</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="0"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -1111,15 +1095,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555551" footer="0.51180555555555551"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555562" footer="0.51180555555555562"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1190,7 +1172,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
@@ -1198,7 +1180,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1208,7 +1190,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1257,7 +1239,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
@@ -1265,7 +1247,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1275,7 +1257,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1598,11 +1580,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1612,7 +1594,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1640,11 +1622,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1654,7 +1636,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1673,15 +1655,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:IU37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="34.28515625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="38.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
@@ -1696,7 +1678,7 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -1715,7 +1697,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -1727,7 +1709,7 @@
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1739,8 +1721,8 @@
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.5" thickBot="1"/>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="47" t="s">
         <v>6</v>
       </c>
@@ -1772,61 +1754,107 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+    <row r="6" spans="1:11" ht="15">
+      <c r="A6" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="16">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16">
+        <v>5</v>
+      </c>
+      <c r="D6" s="17">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0.34166666666666662</v>
+      </c>
+      <c r="F6" s="17">
+        <v>0.34722222222222227</v>
+      </c>
       <c r="G6" s="17">
         <f>F6-E6</f>
+        <v>5.5555555555556468E-3</v>
+      </c>
+      <c r="H6" s="16">
         <v>0</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
       <c r="J6" s="32">
         <f>G6+I6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+        <v>5.5555555555556468E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15">
+      <c r="A7" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="7">
+        <v>80</v>
+      </c>
+      <c r="C7" s="7">
+        <v>107</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.36041666666666666</v>
+      </c>
       <c r="G7" s="8">
         <f>F7-E7</f>
+        <v>1.2500000000000011E-2</v>
+      </c>
+      <c r="H7" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
       <c r="J7" s="19">
         <f>G7+I7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="7"/>
+        <v>1.2500000000000011E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15">
+      <c r="A8" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="7">
+        <v>80</v>
+      </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="D8" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.38194444444444442</v>
+      </c>
       <c r="G8" s="8">
         <f>F8-E8</f>
+        <v>1.7361111111111105E-2</v>
+      </c>
+      <c r="H8" s="7">
         <v>0</v>
       </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
       <c r="J8" s="19">
         <f>G8+I8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <v>1.7361111111111105E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1844,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="22"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -1862,27 +1890,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
       <c r="A11" s="50" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="26">
         <f>SUM(B6:B10)</f>
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="C11" s="26">
         <f>SUM(C6:C10)</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="D11" s="27">
         <f>SUM(D6:D10)</f>
-        <v>0</v>
+        <v>3.2638888888888884E-2</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="27">
         <f>SUM(G6:G10)</f>
-        <v>0</v>
+        <v>3.5416666666666763E-2</v>
       </c>
       <c r="H11" s="28">
         <f>SUM(H6:H10)</f>
@@ -1894,71 +1922,71 @@
       </c>
       <c r="J11" s="30">
         <f>SUM(J6:J10)</f>
-        <v>0</v>
+        <v>3.5416666666666763E-2</v>
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
       <c r="A12" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="21" t="str">
+      <c r="B12" s="21">
         <f>IF(EXACT($C$11, 0),"-",ABS($B$11-$C$11)/$C$11)</f>
-        <v>-</v>
+        <v>0.49107142857142855</v>
       </c>
       <c r="D12" s="5"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="13.5" thickBot="1"/>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
       <c r="A14" s="44" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="45"/>
     </row>
-    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15">
       <c r="A15" s="33" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="34">
         <f>C11</f>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15">
       <c r="A16" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="36" t="str">
+      <c r="B16" s="36">
         <f>IF(EXACT($B$15,0),"-",$B$15/((J11-INT(J11))*24))</f>
-        <v>-</v>
+        <v>131.76470588235259</v>
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
       <c r="A17" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="36" t="str">
+      <c r="B17" s="36">
         <f>IF(EXACT($B$15,0),"-",H11/($B$15/10))</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="C17" s="9"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
       <c r="A18" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="38" t="str">
+      <c r="B18" s="38">
         <f>IF(EXACT($B$15,0),"-",H11/$B$15)</f>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="C18" s="46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="37" t="s">
         <v>24</v>
       </c>
@@ -1968,32 +1996,32 @@
       </c>
       <c r="C19" s="42">
         <f>IF(EXACT(J11,0),5%,B19/J11)</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
       <c r="A20" s="40" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="41">
         <f>G11</f>
-        <v>0</v>
+        <v>3.5416666666666763E-2</v>
       </c>
       <c r="C20" s="43">
         <f>IF(EXACT(J11,0),95%,B20/J11)</f>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="D22" s="6"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4">
       <c r="C35" s="4"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:4">
       <c r="D37" s="4"/>
     </row>
   </sheetData>

</xml_diff>